<commit_message>
interar com o nedejs
</commit_message>
<xml_diff>
--- a/PrimaveraTaskPane-INO/PrimaveraTaskPane/bin/Debug/Book1.xlsx
+++ b/PrimaveraTaskPane-INO/PrimaveraTaskPane/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Ra2fd7c64b936462f"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf985a0da15014974"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="Ra0e09e8b1b4b45d8"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R162b816db3dd49b6"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{894d9456-5b6d-4b24-9c19-ab0079f251b2}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2ed3757c-8bb3-4d67-8372-1dc842193818}">
   <we:reference id="a13a8c45-0d9f-477d-b9a5-809c1d218a04" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Load lists from server NODEJS
Load lists from server NODEJS
</commit_message>
<xml_diff>
--- a/PrimaveraTaskPane-INO/PrimaveraTaskPane/bin/Debug/Book1.xlsx
+++ b/PrimaveraTaskPane-INO/PrimaveraTaskPane/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="Rf985a0da15014974"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R9d6e7c480f984f32"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R162b816db3dd49b6"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R5528a450c5bc47a1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{2ed3757c-8bb3-4d67-8372-1dc842193818}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{1535febe-ccba-428e-89af-831ed0af735b}">
   <we:reference id="a13a8c45-0d9f-477d-b9a5-809c1d218a04" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>

<commit_message>
Alterar o cálculo de formula
</commit_message>
<xml_diff>
--- a/PrimaveraTaskPane-INO/PrimaveraTaskPane/bin/Debug/Book1.xlsx
+++ b/PrimaveraTaskPane-INO/PrimaveraTaskPane/bin/Debug/Book1.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <x:sheets>
-    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R28baa906b40d4f22"/>
+    <x:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="R961a11d2e60d4901"/>
   </x:sheets>
 </x:workbook>
 </file>
@@ -10,13 +10,13 @@
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
   <wetp:taskpane dockstate="" visibility="1" width="350" row="1">
-    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R6b9fd0c4cf394251"/>
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="R22670fdd197b4c82"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
 
 <file path=xl/webextensions/webextension.xml><?xml version="1.0" encoding="utf-8"?>
-<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{061fb1a3-550d-4e8d-abc7-24a384ed0d68}">
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{e694c2eb-cfa4-4e87-8ab4-e0f47a8703d8}">
   <we:reference id="a13a8c45-0d9f-477d-b9a5-809c1d218a04" version="1.0.0.0" store="developer" storeType="Registry"/>
   <we:alternateReferences/>
   <we:properties/>

</xml_diff>